<commit_message>
File path location overhaul
</commit_message>
<xml_diff>
--- a/Data_clustered.xlsx
+++ b/Data_clustered.xlsx
@@ -18219,13 +18219,18 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <TaxCatchAll xmlns="814e9f69-708b-42d1-b772-2ece2c1b39da" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c547a812-ac17-4a6a-8bd9-a75acfa31021">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E412483FFC35649B797435CD3F0398D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc1693a0f8f8a56dd0f8736d468a9701">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c547a812-ac17-4a6a-8bd9-a75acfa31021" xmlns:ns3="814e9f69-708b-42d1-b772-2ece2c1b39da" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dee7b86f1ea803d04819fbf1cdce97f7" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E412483FFC35649B797435CD3F0398D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d1ef06f25ed612914346073c669f3d57">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c547a812-ac17-4a6a-8bd9-a75acfa31021" xmlns:ns3="814e9f69-708b-42d1-b772-2ece2c1b39da" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8df51d0651151a8208a9da934d0771e3" ns2:_="" ns3:_="">
     <xsd:import namespace="c547a812-ac17-4a6a-8bd9-a75acfa31021"/>
     <xsd:import namespace="814e9f69-708b-42d1-b772-2ece2c1b39da"/>
     <xsd:element name="properties">
@@ -18247,6 +18252,8 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -18316,6 +18323,13 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5ec99919-4982-4388-8a64-83a11d2ca210" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="814e9f69-708b-42d1-b772-2ece2c1b39da" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -18345,6 +18359,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c59faeb6-52d7-4144-9b03-0dbc3402ce3f}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="814e9f69-708b-42d1-b772-2ece2c1b39da">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -18465,7 +18490,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{575AA765-A0AC-4C1C-9E6D-57A567A8AEC9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56AEED9E-BB8B-4449-9966-5DF30C46EE00}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>